<commit_message>
Implemented an api gateway for the Company Resource Management Application
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Java Codes\Employee_Details_Operations_Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Employee_Details_Operations_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB574DED-E374-4AD8-8AF3-8E3B6E66A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84726268-62AC-46C1-AB6B-2E71C7EDBE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -161,18 +161,12 @@
     <t xml:space="preserve">Pagination and sorting </t>
   </si>
   <si>
-    <t xml:space="preserve">Skipped . Will have to revisit again after necessities have been fullfilled </t>
-  </si>
-  <si>
     <t xml:space="preserve">mvn clean install </t>
   </si>
   <si>
     <t>mvn clean install -s "%USERPROFILE%\.m2\settings-employee-project.xml"</t>
   </si>
   <si>
-    <t>Cleans the older target file and reinstalls and builds the application from beginning</t>
-  </si>
-  <si>
     <t>Command :</t>
   </si>
   <si>
@@ -186,13 +180,29 @@
   </si>
   <si>
     <t>Bug Solved Date :</t>
+  </si>
+  <si>
+    <t>Skipped . Will have to revisit again after necessities have been fullfilled . 
+Update 1 : Implemented Pagination and tested thoroghly .Implementation Date : 23/06/2025 . Github reference number : 935703f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system agnostic file location </t>
+  </si>
+  <si>
+    <t>../Folder/SubFolder/FileName.file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../ means the 2ns last directory . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleans the older target file and reinstalls and builds the application from beginning using the custom settings.xml file where %USERPROFILE% is just the user profile directory </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +225,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +259,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -283,11 +313,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,7 +364,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,10 +829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,24 +845,35 @@
   <sheetData>
     <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -821,93 +883,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD7B9C-7081-47F2-A303-D50CDA5B6E11}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.6328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="84.08984375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="19.36328125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29" style="13" customWidth="1"/>
+    <col min="5" max="5" width="84.08984375" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:5" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
+        <v>45809</v>
+      </c>
+      <c r="B6" s="14">
+        <v>45831</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed the folder to Company Resource Management Application . Made the folder a maven project . Created a pom.xml , custom settings.xml for build . This is the overall application which will contain other microservices controlled by the api-gateway service
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Java Codes\Employee_Details_Operations_Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Github\Company_Resource_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB574DED-E374-4AD8-8AF3-8E3B6E66A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779DC8B6-01D5-4786-9BE6-A7F37331E94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Bug Solved Date :</t>
+  </si>
+  <si>
+    <t>mvn clean install -s"company_resources_management_application_settings.xml"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleans the older target file and reinstalls and builds the application from beginning when the settings.xml file is present inside the appication folder </t>
   </si>
 </sst>
 </file>
@@ -608,25 +614,25 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="37.54296875" customWidth="1"/>
-    <col min="4" max="5" width="7.90625" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
-    <col min="7" max="7" width="48.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="41.08984375" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="41.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="39" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="C2" s="9" t="s">
         <v>15</v>
@@ -638,7 +644,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -650,7 +656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>12</v>
@@ -662,7 +668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -674,7 +680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="C6" s="8" t="s">
         <v>14</v>
@@ -686,7 +692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
@@ -694,7 +700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
@@ -702,7 +708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
@@ -710,7 +716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
@@ -721,7 +727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
@@ -732,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
@@ -743,29 +749,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:11" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
@@ -778,21 +784,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="57.90625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="88.7265625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="21.36328125" style="5"/>
+    <col min="1" max="1" width="19.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="21.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
@@ -803,7 +809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -812,6 +818,17 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -823,21 +840,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD7B9C-7081-47F2-A303-D50CDA5B6E11}">
   <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.6328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="84.08984375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="18.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="84.140625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
@@ -854,7 +871,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>45809</v>
       </c>
@@ -868,7 +885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>45809</v>
       </c>
@@ -882,7 +899,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>45809</v>
       </c>
@@ -896,7 +913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>45809</v>
       </c>

</xml_diff>

<commit_message>
Updated the information excel sheet
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Github\Company_Resource_Management_Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Employee_Details_Operations_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779DC8B6-01D5-4786-9BE6-A7F37331E94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84726268-62AC-46C1-AB6B-2E71C7EDBE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -161,18 +161,12 @@
     <t xml:space="preserve">Pagination and sorting </t>
   </si>
   <si>
-    <t xml:space="preserve">Skipped . Will have to revisit again after necessities have been fullfilled </t>
-  </si>
-  <si>
     <t xml:space="preserve">mvn clean install </t>
   </si>
   <si>
     <t>mvn clean install -s "%USERPROFILE%\.m2\settings-employee-project.xml"</t>
   </si>
   <si>
-    <t>Cleans the older target file and reinstalls and builds the application from beginning</t>
-  </si>
-  <si>
     <t>Command :</t>
   </si>
   <si>
@@ -188,17 +182,27 @@
     <t>Bug Solved Date :</t>
   </si>
   <si>
-    <t>mvn clean install -s"company_resources_management_application_settings.xml"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleans the older target file and reinstalls and builds the application from beginning when the settings.xml file is present inside the appication folder </t>
+    <t>Skipped . Will have to revisit again after necessities have been fullfilled . 
+Update 1 : Implemented Pagination and tested thoroghly .Implementation Date : 23/06/2025 . Github reference number : 935703f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system agnostic file location </t>
+  </si>
+  <si>
+    <t>../Folder/SubFolder/FileName.file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../ means the 2ns last directory . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleans the older target file and reinstalls and builds the application from beginning using the custom settings.xml file where %USERPROFILE% is just the user profile directory </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,8 +225,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,8 +259,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -289,11 +313,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,7 +364,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,25 +659,25 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
-    <col min="4" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="48.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="41.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" customWidth="1"/>
+    <col min="4" max="5" width="7.90625" customWidth="1"/>
+    <col min="6" max="6" width="5.6328125" customWidth="1"/>
+    <col min="7" max="7" width="48.26953125" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="41.08984375" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="39" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="C2" s="9" t="s">
         <v>15</v>
@@ -644,7 +689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -656,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>12</v>
@@ -668,7 +713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -680,7 +725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="C6" s="8" t="s">
         <v>14</v>
@@ -692,7 +737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
@@ -700,7 +745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
@@ -708,7 +753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
@@ -716,7 +761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
@@ -727,7 +772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
@@ -738,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
@@ -749,29 +794,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
@@ -784,50 +829,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="21.42578125" style="5"/>
+    <col min="1" max="1" width="19.36328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="57.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="88.7265625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="21.36328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -838,93 +883,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD7B9C-7081-47F2-A303-D50CDA5B6E11}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="84.140625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="19.36328125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29" style="13" customWidth="1"/>
+    <col min="5" max="5" width="84.08984375" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:5" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>45809</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
+        <v>45809</v>
+      </c>
+      <c r="B6" s="14">
+        <v>45831</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>45809</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the Department Service package structure . Although for now it's not working since I haven't decided about the service functions , data types and database etc . Will be implementing full version in upcoming commits .
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Employee_Details_Operations_Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Company_Resources_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84726268-62AC-46C1-AB6B-2E71C7EDBE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D117A952-3BCB-4913-AD99-A3DA546A9BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
     <sheet name="commands to remember" sheetId="3" r:id="rId2"/>
     <sheet name="Employee Application Backlogs" sheetId="2" r:id="rId3"/>
+    <sheet name="Api Architecture" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -831,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -979,4 +980,21 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25BFE67-C1D7-4E01-9556-4056E1C4C1E6}">
+  <dimension ref="A22:A25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced mySql database with mongodb database since a lot of information will be in form of lists which will be better to be dealt in mongodb . Currently,/testConnection and /testDataBaseConnection has been implemented and tested . CRUD operations endpoints will be perfected and pushed next time.
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Company_Resources_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D117A952-3BCB-4913-AD99-A3DA546A9BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C20213-AC81-454E-A4E0-BDFBA79E7A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve">    DepartmentName VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Location VARCHAR(100),</t>
   </si>
   <si>
     <t xml:space="preserve">    PRIMARY KEY (DepartmentID)</t>
@@ -197,13 +194,22 @@
   </si>
   <si>
     <t xml:space="preserve">Cleans the older target file and reinstalls and builds the application from beginning using the custom settings.xml file where %USERPROFILE% is just the user profile directory </t>
+  </si>
+  <si>
+    <t>DepartmentHeadId int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Locations List VARCHAR(100),</t>
+  </si>
+  <si>
+    <t>DepartmentEmployeeIds List Int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +246,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -267,7 +280,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -329,11 +342,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,6 +399,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,102 +694,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="37.54296875" customWidth="1"/>
-    <col min="4" max="5" width="7.90625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="3.36328125" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" customWidth="1"/>
     <col min="6" max="6" width="5.6328125" customWidth="1"/>
-    <col min="7" max="7" width="48.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="41.08984375" customWidth="1"/>
+    <col min="7" max="7" width="57.90625" customWidth="1"/>
+    <col min="8" max="8" width="4.26953125" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" customWidth="1"/>
+    <col min="10" max="10" width="53" customWidth="1"/>
     <col min="12" max="12" width="12.6328125" customWidth="1"/>
     <col min="13" max="13" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="68.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="39" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="C2" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+      <c r="C5" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
+      <c r="C6" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -759,23 +804,23 @@
         <v>7</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>8</v>
@@ -786,24 +831,24 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C14" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" s="5"/>
     </row>
@@ -814,17 +859,18 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C16" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -846,35 +892,35 @@
   <sheetData>
     <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -903,19 +949,19 @@
     <row r="1" spans="1:5" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" s="15" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="C2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -926,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -940,10 +986,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -954,10 +1000,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -971,10 +1017,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25BFE67-C1D7-4E01-9556-4056E1C4C1E6}">
   <dimension ref="A22:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replaced mySql database with mongodb database since a lot of information will be in form of lists which will be better to be dealt in mongodb .All CRUD operations including health checks are working properly
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Company_Resources_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C20213-AC81-454E-A4E0-BDFBA79E7A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A79B03B-86DD-4EA8-9645-D4D87F8AD370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3260" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,7 +818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Implemented unit testing for AuthenticationController.java in AuthenticationControllerUnitTest.java . All situations are tested and this reduces manually testing every functionality of AuthenticationController after new technology implementation .
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Company_Resources_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A79B03B-86DD-4EA8-9645-D4D87F8AD370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E8EA27-94CF-4BBB-892B-9564BCB45487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Data records app" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>DepartmentEmployeeIds List Int</t>
+  </si>
+  <si>
+    <t>mvn dtest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mvn test -Dtest=AuthenticationControllerUnitTest</t>
+  </si>
+  <si>
+    <t>it runs the particular test class , here the class is AuthenticationControllerUnitTest</t>
   </si>
 </sst>
 </file>
@@ -694,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -876,10 +885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,6 +930,17 @@
       </c>
       <c r="C3" s="5" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented new exception handling method which handles invalid page number for fetch employee data records
</commit_message>
<xml_diff>
--- a/Company Records Application.xlsx
+++ b/Company Records Application.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emajsab\Github\Company_Resources_Management_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E8EA27-94CF-4BBB-892B-9564BCB45487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14B771C-63B5-4C52-9194-680383ACC24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t xml:space="preserve">    FirstName VARCHAR(50) NOT NULL,</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>it runs the particular test class , here the class is AuthenticationControllerUnitTest</t>
+  </si>
+  <si>
+    <t>mvn clean install -DskipTests</t>
+  </si>
+  <si>
+    <t>clean install with out retesting the application</t>
   </si>
 </sst>
 </file>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411976D6-6315-4CAA-8335-D63811E3A4C2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -941,6 +947,14 @@
       </c>
       <c r="C4" s="5" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>